<commit_message>
added exercise for isi->m2m_device enable
</commit_message>
<xml_diff>
--- a/imx219/exercise-02/readme.xlsx
+++ b/imx219/exercise-02/readme.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="15">
   <si>
     <t xml:space="preserve">Imx8mp-evk-dual-ov2775.dts</t>
   </si>
@@ -79,6 +79,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,12 +168,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E30" activeCellId="0" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="24.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.41"/>
@@ -274,6 +275,9 @@
       <c r="D6" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="E6" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -321,6 +325,9 @@
       </c>
       <c r="D9" s="0" t="s">
         <v>6</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>